<commit_message>
sync: added visited by me and image flags to df
</commit_message>
<xml_diff>
--- a/source/my_trips/Hiking_journal.xlsx
+++ b/source/my_trips/Hiking_journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Nr. stamp</t>
   </si>
@@ -242,6 +242,48 @@
   </si>
   <si>
     <t>HWN026 Mönchsbuche</t>
+  </si>
+  <si>
+    <t>HWN099 Harzer Holzdampflok</t>
+  </si>
+  <si>
+    <t>https://www.komoot.com/de-de/tour/2088114497</t>
+  </si>
+  <si>
+    <t>HWN100 Ebersburg</t>
+  </si>
+  <si>
+    <t>HWN218 Neustädter Talsperre</t>
+  </si>
+  <si>
+    <t>HWN098 Ruine Hohnstein</t>
+  </si>
+  <si>
+    <t>HWN164 Stiefmutter</t>
+  </si>
+  <si>
+    <t>https://www.komoot.com/de-de/tour/2112900887</t>
+  </si>
+  <si>
+    <t>HWN165 Wendel-Eiche</t>
+  </si>
+  <si>
+    <t>HWN090 Roter Schuss</t>
+  </si>
+  <si>
+    <t>HWN035 Gasthaus Armeleuteberg</t>
+  </si>
+  <si>
+    <t>https://www.komoot.com/de-de/tour/2021000530</t>
+  </si>
+  <si>
+    <t>HWN034 Scharfenstein</t>
+  </si>
+  <si>
+    <t>HWN032 Gasthaus Christianental</t>
+  </si>
+  <si>
+    <t>HWN031 Agnesberg</t>
   </si>
 </sst>
 </file>
@@ -584,14 +626,14 @@
       </c>
       <c r="E1" s="3">
         <f>SUM(E2:E126)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3">
         <f>COUNTA(A2:A250)</f>
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
@@ -1306,8 +1348,147 @@
         <v>45676.0</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="4">
+        <v>45724.0</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="4">
+        <v>45724.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>218.0</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="4">
+        <v>45724.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>98.0</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="4">
+        <v>45724.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>164.0</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="4">
+        <v>45739.0</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>165.0</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="4">
+        <v>45739.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>90.0</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="4">
+        <v>45739.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="4">
+        <v>45778.0</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="4">
+        <v>45778.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>32.0</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="4">
+        <v>45778.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>31.0</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="4">
+        <v>45778.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="34">
     <mergeCell ref="D4:D7"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="D8:D10"/>
@@ -1326,9 +1507,15 @@
     <mergeCell ref="D46:D49"/>
     <mergeCell ref="D50:D53"/>
     <mergeCell ref="D54:D57"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D65:D68"/>
     <mergeCell ref="E46:E49"/>
     <mergeCell ref="E50:E53"/>
     <mergeCell ref="E54:E57"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="E65:E68"/>
     <mergeCell ref="D32:D34"/>
     <mergeCell ref="E32:E34"/>
     <mergeCell ref="D35:D37"/>
@@ -1354,7 +1541,10 @@
     <hyperlink r:id="rId14" ref="D46"/>
     <hyperlink r:id="rId15" ref="D50"/>
     <hyperlink r:id="rId16" ref="D54"/>
+    <hyperlink r:id="rId17" ref="D58"/>
+    <hyperlink r:id="rId18" ref="D62"/>
+    <hyperlink r:id="rId19" ref="D65"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>